<commit_message>
SenderBot run msg sender logic; utils get_datetime_passed_seconds
</commit_message>
<xml_diff>
--- a/assets/users.xlsx
+++ b/assets/users.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="53">
   <si>
     <t>Место проведения уборки</t>
   </si>
@@ -31,10 +31,13 @@
     <t>Кирилл Александрович</t>
   </si>
   <si>
-    <t>Ежедневно в 13:30 по рем.зоне. Ежедневно в 19:30 по магазину</t>
+    <t>Ежедневно в 13:30 по рем.зоне.</t>
   </si>
   <si>
     <t>Космонавтов 73</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ежедневно в 19:30 по магазину </t>
   </si>
   <si>
     <t>Альберта Камалеева 44</t>
@@ -499,9 +502,11 @@
       <c r="C2" s="3">
         <v>8.9172507133E10</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
@@ -513,291 +518,295 @@
       <c r="C3" s="3">
         <v>8.9172507133E10</v>
       </c>
+      <c r="D3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="4"/>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4" s="3">
         <v>8.9172751878E10</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" s="5">
         <f>89274151717</f>
         <v>89274151717</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C6" s="3">
         <v>8.9083308828E10</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C7" s="3">
         <v>8.91968533E10</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C8" s="3">
         <v>8.9510652494E10</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C9" s="3">
         <v>8.9520479512E10</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C10" s="8">
         <v>8.9172855795E10</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C11" s="8">
         <v>8.9874116242E10</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C12" s="8">
         <v>8.9274316881E10</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C13" s="8">
         <v>8.9503115888E10</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C14" s="8">
         <v>8.9375877708E10</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="8" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C15" s="8">
         <v>8.937772278E10</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C16" s="8">
         <v>8.9272424735E10</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="8" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C17" s="8">
         <v>8.9874138419E10</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C18" s="8">
         <v>8.937770615E10</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C19" s="8">
         <v>8.9172560722E10</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="8" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C20" s="8">
         <v>8.9503198764E10</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C21" s="8">
         <v>8.9503155177E10</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C22" s="8">
         <v>8.9053168294E10</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C23" s="8">
         <v>8.9129467815E10</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>